<commit_message>
updates to calculator spreadsheet
</commit_message>
<xml_diff>
--- a/clientdocs/Mike calculator v2.xlsx
+++ b/clientdocs/Mike calculator v2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27810" windowHeight="12195" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27810" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="MDM calculator" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="258">
   <si>
     <t>Medical Decision Making - Problems being addressed, data being reviewed, risk to patient.</t>
   </si>
@@ -889,6 +889,15 @@
   </si>
   <si>
     <t>family history</t>
+  </si>
+  <si>
+    <t>tetste</t>
+  </si>
+  <si>
+    <t>est problem</t>
+  </si>
+  <si>
+    <t>stable problem</t>
   </si>
 </sst>
 </file>
@@ -2284,7 +2293,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2295,7 +2304,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2330,7 +2339,7 @@
       <c r="L1" s="130"/>
       <c r="N1" s="132" t="str">
         <f>"CC: "&amp;E1&amp;" Problems addressed in this encounter include "&amp;F9&amp;G9&amp;F10&amp;G10&amp;F12&amp;G12&amp;F13&amp;G13&amp;F14&amp;G14&amp;F15&amp;G15&amp;F16&amp;G16&amp;F18&amp;G18&amp;F19&amp;G19&amp;F20&amp;G20&amp;F21&amp;G21&amp;F22&amp;G22&amp;F24&amp;G24&amp;F26&amp;K26&amp;F27&amp;K27&amp;F28&amp;K28&amp;F29&amp;K29&amp;F30&amp;K30&amp;"."&amp;"Additional workup planned (if any), includes: "&amp;G26&amp;K26&amp;G27&amp;K27&amp;G28&amp;K28&amp;G29&amp;K29&amp;G30&amp;K30&amp;"."&amp;K36&amp;K37&amp;K38&amp;K39&amp;K40&amp;K41&amp;"Risk to patient is considered "&amp;F49&amp;" due to "&amp;G49&amp;"."</f>
-        <v>CC:  Problems addressed in this encounter include .Additional workup planned (if any), includes: .Risk to patient is considered Minimal due to having only one minor (self-limiting) problem.</v>
+        <v>CC:  Problems addressed in this encounter include est problem, stable problem, .Additional workup planned (if any), includes: .Risk to patient is considered Moderate due to stopping, starting, or changing Rx (other than LiCo).</v>
       </c>
       <c r="O1" s="132"/>
       <c r="P1" s="132"/>
@@ -2584,14 +2593,16 @@
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>256</v>
+      </c>
       <c r="G12" s="128" t="str">
         <f t="shared" ref="G12:G24" si="0" xml:space="preserve"> IF(ISTEXT(F12),", ","")</f>
-        <v/>
+        <v xml:space="preserve">, </v>
       </c>
       <c r="H12" s="27">
         <f xml:space="preserve"> IF(ISTEXT(F12),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="64" t="s">
         <v>230</v>
@@ -2609,14 +2620,16 @@
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>257</v>
+      </c>
       <c r="G13" s="128" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v xml:space="preserve">, </v>
       </c>
       <c r="H13" s="27">
         <f xml:space="preserve"> IF(ISTEXT(F13),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="64" t="s">
         <v>231</v>
@@ -2987,7 +3000,7 @@
       <c r="E31" s="13"/>
       <c r="H31" s="15">
         <f>SUM(H9:H30)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -3218,10 +3231,10 @@
       <c r="D49" s="13"/>
       <c r="F49" s="13" t="str">
         <f>VLOOKUP(G49,ki,2,FALSE)</f>
-        <v>Minimal</v>
+        <v>Moderate</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -3468,8 +3481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A184" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A207" sqref="A207:G223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -5668,7 +5681,7 @@
         <v>70</v>
       </c>
       <c r="B115" s="29"/>
-      <c r="C115" s="105"/>
+      <c r="C115" s="106"/>
       <c r="D115" s="56"/>
       <c r="E115" s="56"/>
       <c r="F115" s="22">
@@ -7253,12 +7266,17 @@
       <c r="D196" s="22"/>
       <c r="E196" s="22"/>
       <c r="F196" s="22"/>
-      <c r="G196" s="97"/>
+      <c r="G196" s="97" t="str">
+        <f xml:space="preserve"> IF(ISTEXT(B196),C196&amp;"/","")</f>
+        <v/>
+      </c>
     </row>
     <row r="197" spans="1:7">
       <c r="A197" s="43"/>
       <c r="B197" s="101"/>
-      <c r="C197" s="112"/>
+      <c r="C197" s="112" t="s">
+        <v>255</v>
+      </c>
       <c r="D197" s="22"/>
       <c r="E197" s="22"/>
       <c r="F197" s="22"/>
@@ -7347,7 +7365,7 @@
     <row r="207" spans="1:7" ht="180" customHeight="1">
       <c r="A207" s="133" t="str">
         <f>'MDM calculator'!N1&amp;G1&amp;"-----HPI: "&amp;G11&amp;" "&amp;G12&amp;" "&amp;G13&amp;" "&amp;G14&amp;" "&amp;G15&amp;" "&amp;G16&amp;" "&amp;G17&amp;" "&amp;G18&amp;"-----PFSH: MEDICAL HISTORY:"&amp;G23&amp;"-----FH:"&amp;G25&amp;" "&amp;G26&amp;" "&amp;G27&amp;" "&amp;G28&amp;" "&amp;G29&amp;" "&amp;G30&amp;" "&amp;G31&amp;" "&amp;G32&amp;" "&amp;G33&amp;" "&amp;G34&amp;" "&amp;G35&amp;" "&amp;G36&amp;"-----SH: "&amp;G38&amp;" "&amp;G39&amp;" "&amp;G40&amp;" "&amp;G41&amp;" "&amp;G42&amp;" "&amp;G43&amp;" "&amp;G44&amp;" "&amp;G45&amp;" "&amp;G46&amp;" "&amp;G47&amp;"-----ROS: "&amp;G53&amp;" "&amp;G54&amp;" "&amp;G55&amp;" "&amp;G56&amp;" "&amp;G57&amp;" "&amp;G58&amp;" "&amp;G60&amp;" "&amp;G61&amp;" "&amp;G62&amp;" "&amp;G63&amp;" "&amp;G64&amp;" "&amp;G65&amp;" "&amp;G66&amp;" "&amp;G68&amp;" "&amp;G69&amp;" "&amp;G70&amp;" "&amp;G72&amp;" "&amp;G73&amp;" "&amp;G74&amp;" "&amp;G75&amp;" "&amp;G77&amp;" "&amp;G78&amp;" "&amp;G79&amp;" "&amp;G80&amp;" "&amp;G81&amp;" "&amp;G83&amp;" "&amp;G84&amp;" "&amp;G85&amp;" "&amp;G86&amp;" "&amp;G87&amp;" "&amp;G89&amp;" "&amp;G91&amp;" "&amp;G93&amp;" "&amp;G95&amp;" "&amp;G97&amp;" "&amp;G99&amp;" "&amp;G101&amp;" "&amp;G103&amp;" "&amp;G104&amp;"-----EXAM: "&amp;G123&amp;" "&amp;G124&amp;" "&amp;G125&amp;" "&amp;G127&amp;" "&amp;G128&amp;" "&amp;G129&amp;" "&amp;G131&amp;" "&amp;G141&amp;" "&amp;G154&amp;" "&amp;G157&amp;" "&amp;G158&amp;" "&amp;G163&amp;" "&amp;G165&amp;" "&amp;G167&amp;" "&amp;G169&amp;" "&amp;G171&amp;" "&amp;G173&amp;" "&amp;G175&amp;" "&amp;G177&amp;"----------"&amp;G186&amp;G187&amp;G188&amp;"  Psychotherapy included: "&amp;G191&amp;" "&amp;G192&amp;" "&amp;G193&amp;" "&amp;G194&amp;" "&amp;G195&amp;" "&amp;G197&amp;"."</f>
-        <v>CC:  Problems addressed in this encounter include .Additional workup planned (if any), includes: .Risk to patient is considered Minimal due to having only one minor (self-limiting) problem.MDM is High.-----HPI: Pt. has had sadness for long time.   Associated signs/symptoms include lots of signs. Timing is constant. The symptoms are severe. The symptoms occur in the context of all the time. Modifying factors:everything. Location in body:everywhere. Quality:bad.-----PFSH: MEDICAL HISTORY:complete medical info-----FH:family history Mother:none. Father:none. Maternal grandmother:none. Maternal grandfather:none. Paternal grandmother:none. Paternal grandfather:none. Sibling 1:none. Sibling 2:none. Sibling 3:none. Sibling 4:none. Other family member:none.-----SH: social issues Has a job. Has a car. C-section birth. Has not has gallbladder removed. Has had gastric bypass surgery. No developmental delays. Learned to read at young age. Furthest educational level: college degree. Housing: owns home.-----ROS: Negative for hallucinations. Negative for SI. Negative for anxiety. Negative for insomnia. Negative for drug/alcohol abuse.  Constitutional:Negative for fatigue.              GI:Negative for nausea.                  All other systems reviewed and are negative.-----EXAM:    Inappropriately groomed and/or dressed PLEASE OVERRIDE TEXT HERE TO EXPLAIN Pt. has nutritional deficiencies. PLEASE OVERRIDE TEXT HERE TO EXPLAIN Has deformities relevant to mental status. OVERRIDE TEXT HERE TO EXPLAIN Speech is normal for  Thought content: . Associations are loose. Pt. confirms . Pt. denies SI/HI, hallucinations, delusions, obsessions, aggressive/violent ruminations.. Loose judgment/insight. OVERIDE TEXT HERE TO ELABORATE Recent and remote memory is loose. Attention span/concentration below average. OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE. Mood is , and affect congruent.----------  Psychotherapy included:      .</v>
+        <v>CC:  Problems addressed in this encounter include est problem, stable problem, .Additional workup planned (if any), includes: .Risk to patient is considered Moderate due to stopping, starting, or changing Rx (other than LiCo).MDM is High.-----HPI: Pt. has had sadness for long time.   Associated signs/symptoms include lots of signs. Timing is constant. The symptoms are severe. The symptoms occur in the context of all the time. Modifying factors:everything. Location in body:everywhere. Quality:bad.-----PFSH: MEDICAL HISTORY:complete medical info-----FH:family history Mother:none. Father:none. Maternal grandmother:none. Maternal grandfather:none. Paternal grandmother:none. Paternal grandfather:none. Sibling 1:none. Sibling 2:none. Sibling 3:none. Sibling 4:none. Other family member:none.-----SH: social issues Has a job. Has a car. C-section birth. Has not has gallbladder removed. Has had gastric bypass surgery. No developmental delays. Learned to read at young age. Furthest educational level: college degree. Housing: owns home.-----ROS: Negative for hallucinations. Negative for SI. Negative for anxiety. Negative for insomnia. Negative for drug/alcohol abuse.  Constitutional:Negative for fatigue.              GI:Negative for nausea.                  All other systems reviewed and are negative.-----EXAM:    Inappropriately groomed and/or dressed PLEASE OVERRIDE TEXT HERE TO EXPLAIN Pt. has nutritional deficiencies. PLEASE OVERRIDE TEXT HERE TO EXPLAIN Has deformities relevant to mental status. OVERRIDE TEXT HERE TO EXPLAIN Speech is normal for  Thought content: . Associations are loose. Pt. confirms . Pt. denies SI/HI, hallucinations, delusions, obsessions, aggressive/violent ruminations.. Loose judgment/insight. OVERIDE TEXT HERE TO ELABORATE Recent and remote memory is loose. Attention span/concentration below average. OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE. Mood is , and affect congruent.----------  Psychotherapy included:      .</v>
       </c>
       <c r="B207" s="133"/>
       <c r="C207" s="133"/>
@@ -7501,7 +7519,6 @@
       <c r="G223" s="133"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="7">
     <mergeCell ref="A207:G223"/>
     <mergeCell ref="A7:G7"/>
@@ -7563,7 +7580,9 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:P223"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
@@ -11378,7 +11397,7 @@
     <row r="207" spans="1:7" ht="180" customHeight="1">
       <c r="A207" s="133" t="str">
         <f>'MDM calculator'!N1&amp;G1&amp;"-----HPI: "&amp;G11&amp;" "&amp;G12&amp;" "&amp;G13&amp;" "&amp;G14&amp;" "&amp;G15&amp;" "&amp;G16&amp;" "&amp;G17&amp;" "&amp;G18&amp;"-----PFSH: MEDICAL HISTORY:"&amp;G23&amp;"-----FH:"&amp;G25&amp;" "&amp;G26&amp;" "&amp;G27&amp;" "&amp;G28&amp;" "&amp;G29&amp;" "&amp;G30&amp;" "&amp;G31&amp;" "&amp;G32&amp;" "&amp;G33&amp;" "&amp;G34&amp;" "&amp;G35&amp;" "&amp;G36&amp;"-----SH: "&amp;G38&amp;" "&amp;G39&amp;" "&amp;G40&amp;" "&amp;G41&amp;" "&amp;G42&amp;" "&amp;G43&amp;" "&amp;G44&amp;" "&amp;G45&amp;" "&amp;G46&amp;" "&amp;G47&amp;"-----ROS: "&amp;G53&amp;" "&amp;G54&amp;" "&amp;G55&amp;" "&amp;G56&amp;" "&amp;G57&amp;" "&amp;G58&amp;" "&amp;G60&amp;" "&amp;G61&amp;" "&amp;G62&amp;" "&amp;G63&amp;" "&amp;G64&amp;" "&amp;G65&amp;" "&amp;G66&amp;" "&amp;G68&amp;" "&amp;G69&amp;" "&amp;G70&amp;" "&amp;G72&amp;" "&amp;G73&amp;" "&amp;G74&amp;" "&amp;G75&amp;" "&amp;G77&amp;" "&amp;G78&amp;" "&amp;G79&amp;" "&amp;G80&amp;" "&amp;G81&amp;" "&amp;G83&amp;" "&amp;G84&amp;" "&amp;G85&amp;" "&amp;G86&amp;" "&amp;G87&amp;" "&amp;G89&amp;" "&amp;G91&amp;" "&amp;G93&amp;" "&amp;G95&amp;" "&amp;G97&amp;" "&amp;G99&amp;" "&amp;G101&amp;" "&amp;G103&amp;" "&amp;G104&amp;"-----EXAM: "&amp;G123&amp;" "&amp;G124&amp;" "&amp;G125&amp;" "&amp;G127&amp;" "&amp;G128&amp;" "&amp;G129&amp;" "&amp;G131&amp;" "&amp;G141&amp;" "&amp;G154&amp;" "&amp;G157&amp;" "&amp;G158&amp;" "&amp;G163&amp;" "&amp;G165&amp;" "&amp;G167&amp;" "&amp;G169&amp;" "&amp;G171&amp;" "&amp;G173&amp;" "&amp;G175&amp;" "&amp;G177&amp;"----------"&amp;G186&amp;G187&amp;G188&amp;"  Psychotherapy included: "&amp;G191&amp;" "&amp;G192&amp;" "&amp;G193&amp;" "&amp;G194&amp;" "&amp;G195&amp;" "&amp;G197&amp;"."</f>
-        <v>CC:  Problems addressed in this encounter include .Additional workup planned (if any), includes: .Risk to patient is considered Minimal due to having only one minor (self-limiting) problem.MDM is Moderate.-----HPI: Pt. has had  for .         -----PFSH: MEDICAL HISTORY:0-----FH:0           -----SH: 0 Does not have a job. Does not have a car. Not born by C-section or does not know. Gallbladder has been removed. Has not had gastric bypass surgery. No developmental delays. PLEASE ELABORATE  -----ROS: Negative for hallucinations. Negative for SI. Negative for anxiety. Negative for insomnia. Negative for drug/alcohol abuse.  Constitutional:Negative for fatigue.              GI:Negative for nausea.                  All other systems reviewed and are negative.-----EXAM:    Inappropriately groomed and/or dressed PLEASE OVERRIDE TEXT HERE TO EXPLAIN Pt. has nutritional deficiencies. PLEASE OVERRIDE TEXT HERE TO EXPLAIN Has deformities relevant to mental status. OVERRIDE TEXT HERE TO EXPLAIN Speech is normal for  Thought content: . Associations are loose. Pt. confirms . Pt. denies SI/HI, hallucinations, delusions, obsessions, aggressive/violent ruminations.. Loose judgment/insight. OVERIDE TEXT HERE TO ELABORATE Recent and remote memory is loose. Attention span/concentration below average. OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE. Mood is , and affect congruent.----------  Psychotherapy included:      .</v>
+        <v>CC:  Problems addressed in this encounter include est problem, stable problem, .Additional workup planned (if any), includes: .Risk to patient is considered Moderate due to stopping, starting, or changing Rx (other than LiCo).MDM is Moderate.-----HPI: Pt. has had  for .         -----PFSH: MEDICAL HISTORY:0-----FH:0           -----SH: 0 Does not have a job. Does not have a car. Not born by C-section or does not know. Gallbladder has been removed. Has not had gastric bypass surgery. No developmental delays. PLEASE ELABORATE  -----ROS: Negative for hallucinations. Negative for SI. Negative for anxiety. Negative for insomnia. Negative for drug/alcohol abuse.  Constitutional:Negative for fatigue.              GI:Negative for nausea.                  All other systems reviewed and are negative.-----EXAM:    Inappropriately groomed and/or dressed PLEASE OVERRIDE TEXT HERE TO EXPLAIN Pt. has nutritional deficiencies. PLEASE OVERRIDE TEXT HERE TO EXPLAIN Has deformities relevant to mental status. OVERRIDE TEXT HERE TO EXPLAIN Speech is normal for  Thought content: . Associations are loose. Pt. confirms . Pt. denies SI/HI, hallucinations, delusions, obsessions, aggressive/violent ruminations.. Loose judgment/insight. OVERIDE TEXT HERE TO ELABORATE Recent and remote memory is loose. Attention span/concentration below average. OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE. Mood is , and affect congruent.----------  Psychotherapy included:      .</v>
       </c>
       <c r="B207" s="133"/>
       <c r="C207" s="133"/>
@@ -11593,7 +11612,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P223"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
@@ -15488,7 +15509,7 @@
     <row r="207" spans="1:7" ht="180" customHeight="1">
       <c r="A207" s="133" t="str">
         <f>'MDM calculator'!N1&amp;G1&amp;"-----HPI: "&amp;G11&amp;" "&amp;G12&amp;" "&amp;G13&amp;" "&amp;G14&amp;" "&amp;G15&amp;" "&amp;G16&amp;" "&amp;G17&amp;" "&amp;G18&amp;"-----PFSH: MEDICAL HISTORY:"&amp;G23&amp;"-----FH:"&amp;G25&amp;" "&amp;G26&amp;" "&amp;G27&amp;" "&amp;G28&amp;" "&amp;G29&amp;" "&amp;G30&amp;" "&amp;G31&amp;" "&amp;G32&amp;" "&amp;G33&amp;" "&amp;G34&amp;" "&amp;G35&amp;" "&amp;G36&amp;"-----SH: "&amp;G38&amp;" "&amp;G39&amp;" "&amp;G40&amp;" "&amp;G41&amp;" "&amp;G42&amp;" "&amp;G43&amp;" "&amp;G44&amp;" "&amp;G45&amp;" "&amp;G46&amp;" "&amp;G47&amp;"-----ROS: "&amp;G53&amp;" "&amp;G54&amp;" "&amp;G55&amp;" "&amp;G56&amp;" "&amp;G57&amp;" "&amp;G58&amp;" "&amp;G60&amp;" "&amp;G61&amp;" "&amp;G62&amp;" "&amp;G63&amp;" "&amp;G64&amp;" "&amp;G65&amp;" "&amp;G66&amp;" "&amp;G68&amp;" "&amp;G69&amp;" "&amp;G70&amp;" "&amp;G72&amp;" "&amp;G73&amp;" "&amp;G74&amp;" "&amp;G75&amp;" "&amp;G77&amp;" "&amp;G78&amp;" "&amp;G79&amp;" "&amp;G80&amp;" "&amp;G81&amp;" "&amp;G83&amp;" "&amp;G84&amp;" "&amp;G85&amp;" "&amp;G86&amp;" "&amp;G87&amp;" "&amp;G89&amp;" "&amp;G91&amp;" "&amp;G93&amp;" "&amp;G95&amp;" "&amp;G97&amp;" "&amp;G99&amp;" "&amp;G101&amp;" "&amp;G103&amp;" "&amp;G104&amp;"-----EXAM: "&amp;G123&amp;" "&amp;G124&amp;" "&amp;G125&amp;" "&amp;G127&amp;" "&amp;G128&amp;" "&amp;G129&amp;" "&amp;G131&amp;" "&amp;G141&amp;" "&amp;G154&amp;" "&amp;G157&amp;" "&amp;G158&amp;" "&amp;G163&amp;" "&amp;G165&amp;" "&amp;G167&amp;" "&amp;G169&amp;" "&amp;G171&amp;" "&amp;G173&amp;" "&amp;G175&amp;" "&amp;G177&amp;"----------"&amp;G186&amp;G187&amp;G188&amp;"  Psychotherapy included: "&amp;G191&amp;" "&amp;G192&amp;" "&amp;G193&amp;" "&amp;G194&amp;" "&amp;G195&amp;" "&amp;G197&amp;"."</f>
-        <v>CC:  Problems addressed in this encounter include .Additional workup planned (if any), includes: .Risk to patient is considered Minimal due to having only one minor (self-limiting) problem.MDM is Low.-----HPI: Pt. has had  for .         -----PFSH: MEDICAL HISTORY:0-----FH:0           -----SH: 0 Does not have a job. Does not have a car. Not born by C-section or does not know. Gallbladder has been removed. Has not had gastric bypass surgery. No developmental delays. PLEASE ELABORATE  -----ROS: Negative for hallucinations. Negative for SI. Negative for anxiety. Negative for insomnia. Negative for drug/alcohol abuse.  Constitutional:Negative for fatigue.              GI:Negative for nausea.                  All other systems reviewed and are negative.-----EXAM:    Inappropriately groomed and/or dressed PLEASE OVERRIDE TEXT HERE TO EXPLAIN Pt. has nutritional deficiencies. PLEASE OVERRIDE TEXT HERE TO EXPLAIN Has deformities relevant to mental status. OVERRIDE TEXT HERE TO EXPLAIN Speech is normal for  Thought content: . Associations are loose. Pt. confirms . Pt. denies SI/HI, hallucinations, delusions, obsessions, aggressive/violent ruminations.. Loose judgment/insight. OVERIDE TEXT HERE TO ELABORATE Recent and remote memory is loose. Attention span/concentration below average. OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE. ----------  Psychotherapy included:      .</v>
+        <v>CC:  Problems addressed in this encounter include est problem, stable problem, .Additional workup planned (if any), includes: .Risk to patient is considered Moderate due to stopping, starting, or changing Rx (other than LiCo).MDM is Low.-----HPI: Pt. has had  for .         -----PFSH: MEDICAL HISTORY:0-----FH:0           -----SH: 0 Does not have a job. Does not have a car. Not born by C-section or does not know. Gallbladder has been removed. Has not had gastric bypass surgery. No developmental delays. PLEASE ELABORATE  -----ROS: Negative for hallucinations. Negative for SI. Negative for anxiety. Negative for insomnia. Negative for drug/alcohol abuse.  Constitutional:Negative for fatigue.              GI:Negative for nausea.                  All other systems reviewed and are negative.-----EXAM:    Inappropriately groomed and/or dressed PLEASE OVERRIDE TEXT HERE TO EXPLAIN Pt. has nutritional deficiencies. PLEASE OVERRIDE TEXT HERE TO EXPLAIN Has deformities relevant to mental status. OVERRIDE TEXT HERE TO EXPLAIN Speech is normal for  Thought content: . Associations are loose. Pt. confirms . Pt. denies SI/HI, hallucinations, delusions, obsessions, aggressive/violent ruminations.. Loose judgment/insight. OVERIDE TEXT HERE TO ELABORATE Recent and remote memory is loose. Attention span/concentration below average. OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE. ----------  Psychotherapy included:      .</v>
       </c>
       <c r="B207" s="133"/>
       <c r="C207" s="133"/>
@@ -15642,7 +15663,6 @@
       <c r="G223" s="133"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="7">
     <mergeCell ref="A207:G223"/>
     <mergeCell ref="A7:G7"/>
@@ -15703,7 +15723,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P223"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
@@ -19595,7 +19617,7 @@
     <row r="207" spans="1:7" ht="180" customHeight="1">
       <c r="A207" s="133" t="str">
         <f>'MDM calculator'!N1&amp;G1&amp;"-----HPI: "&amp;G11&amp;" "&amp;G12&amp;" "&amp;G13&amp;" "&amp;G14&amp;" "&amp;G15&amp;" "&amp;G16&amp;" "&amp;G17&amp;" "&amp;G18&amp;"-----PFSH: MEDICAL HISTORY:"&amp;G23&amp;"-----FH:"&amp;G25&amp;" "&amp;G26&amp;" "&amp;G27&amp;" "&amp;G28&amp;" "&amp;G29&amp;" "&amp;G30&amp;" "&amp;G31&amp;" "&amp;G32&amp;" "&amp;G33&amp;" "&amp;G34&amp;" "&amp;G35&amp;" "&amp;G36&amp;"-----SH: "&amp;G38&amp;" "&amp;G39&amp;" "&amp;G40&amp;" "&amp;G41&amp;" "&amp;G42&amp;" "&amp;G43&amp;" "&amp;G44&amp;" "&amp;G45&amp;" "&amp;G46&amp;" "&amp;G47&amp;"-----ROS: "&amp;G53&amp;" "&amp;G54&amp;" "&amp;G55&amp;" "&amp;G56&amp;" "&amp;G57&amp;" "&amp;G58&amp;" "&amp;G60&amp;" "&amp;G61&amp;" "&amp;G62&amp;" "&amp;G63&amp;" "&amp;G64&amp;" "&amp;G65&amp;" "&amp;G66&amp;" "&amp;G68&amp;" "&amp;G69&amp;" "&amp;G70&amp;" "&amp;G72&amp;" "&amp;G73&amp;" "&amp;G74&amp;" "&amp;G75&amp;" "&amp;G77&amp;" "&amp;G78&amp;" "&amp;G79&amp;" "&amp;G80&amp;" "&amp;G81&amp;" "&amp;G83&amp;" "&amp;G84&amp;" "&amp;G85&amp;" "&amp;G86&amp;" "&amp;G87&amp;" "&amp;G89&amp;" "&amp;G91&amp;" "&amp;G93&amp;" "&amp;G95&amp;" "&amp;G97&amp;" "&amp;G99&amp;" "&amp;G101&amp;" "&amp;G103&amp;" "&amp;G104&amp;"-----EXAM: "&amp;G123&amp;" "&amp;G124&amp;" "&amp;G125&amp;" "&amp;G127&amp;" "&amp;G128&amp;" "&amp;G129&amp;" "&amp;G131&amp;" "&amp;G141&amp;" "&amp;G154&amp;" "&amp;G157&amp;" "&amp;G158&amp;" "&amp;G163&amp;" "&amp;G165&amp;" "&amp;G167&amp;" "&amp;G169&amp;" "&amp;G171&amp;" "&amp;G173&amp;" "&amp;G175&amp;" "&amp;G177&amp;"----------"&amp;G186&amp;G187&amp;G188&amp;"  Psychotherapy included: "&amp;G191&amp;" "&amp;G192&amp;" "&amp;G193&amp;" "&amp;G194&amp;" "&amp;G195&amp;" "&amp;G197&amp;"."</f>
-        <v>CC:  Problems addressed in this encounter include .Additional workup planned (if any), includes: .Risk to patient is considered Minimal due to having only one minor (self-limiting) problem.MDM is Straightforward.-----HPI: Pt. has had  for .         -----PFSH: MEDICAL HISTORY:0-----FH:0           -----SH: 0 Does not have a job. Does not have a car. Not born by C-section or does not know. Gallbladder has been removed. Has not had gastric bypass surgery. No developmental delays. PLEASE ELABORATE  -----ROS: Negative for hallucinations. Negative for SI. Negative for anxiety. Negative for insomnia. Negative for drug/alcohol abuse.  Constitutional:Negative for fatigue.              GI:Negative for nausea.                  All other systems reviewed and are negative.-----EXAM:    Inappropriately groomed and/or dressed PLEASE OVERRIDE TEXT HERE TO EXPLAIN Pt. has nutritional deficiencies. PLEASE OVERRIDE TEXT HERE TO EXPLAIN Has deformities relevant to mental status. OVERRIDE TEXT HERE TO EXPLAIN Speech is normal for  Thought content: . Associations are loose. Pt. confirms . Pt. denies SI/HI, hallucinations, delusions, obsessions, aggressive/violent ruminations.. Loose judgment/insight. OVERIDE TEXT HERE TO ELABORATE Recent and remote memory is loose. Attention span/concentration below average. OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE. ----------  Psychotherapy included:      .</v>
+        <v>CC:  Problems addressed in this encounter include est problem, stable problem, .Additional workup planned (if any), includes: .Risk to patient is considered Moderate due to stopping, starting, or changing Rx (other than LiCo).MDM is Straightforward.-----HPI: Pt. has had  for .         -----PFSH: MEDICAL HISTORY:0-----FH:0           -----SH: 0 Does not have a job. Does not have a car. Not born by C-section or does not know. Gallbladder has been removed. Has not had gastric bypass surgery. No developmental delays. PLEASE ELABORATE  -----ROS: Negative for hallucinations. Negative for SI. Negative for anxiety. Negative for insomnia. Negative for drug/alcohol abuse.  Constitutional:Negative for fatigue.              GI:Negative for nausea.                  All other systems reviewed and are negative.-----EXAM:    Inappropriately groomed and/or dressed PLEASE OVERRIDE TEXT HERE TO EXPLAIN Pt. has nutritional deficiencies. PLEASE OVERRIDE TEXT HERE TO EXPLAIN Has deformities relevant to mental status. OVERRIDE TEXT HERE TO EXPLAIN Speech is normal for  Thought content: . Associations are loose. Pt. confirms . Pt. denies SI/HI, hallucinations, delusions, obsessions, aggressive/violent ruminations.. Loose judgment/insight. OVERIDE TEXT HERE TO ELABORATE Recent and remote memory is loose. Attention span/concentration below average. OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE. ----------  Psychotherapy included:      .</v>
       </c>
       <c r="B207" s="133"/>
       <c r="C207" s="133"/>
@@ -19809,7 +19831,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P238"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A120" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A123" sqref="A123"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -23961,7 +23985,7 @@
     <row r="222" spans="1:16" s="39" customFormat="1" ht="180" customHeight="1">
       <c r="A222" s="133" t="str">
         <f>'MDM calculator'!N1&amp;G1&amp;"-----HPI: "&amp;G21&amp;" "&amp;G22&amp;" "&amp;G23&amp;" "&amp;G24&amp;" "&amp;G25&amp;" "&amp;G26&amp;" "&amp;G27&amp;" "&amp;G28&amp;"-----PFSH: MEDICAL HISTORY:"&amp;C11&amp;":"&amp;G11&amp;"."&amp;C12&amp;":"&amp;G12&amp;"."&amp;C13&amp;":"&amp;G13&amp;"."&amp;G33&amp;"-----FH:"&amp;G35&amp;" "&amp;G36&amp;" "&amp;G37&amp;" "&amp;G38&amp;" "&amp;G39&amp;" "&amp;G40&amp;" "&amp;G41&amp;" "&amp;G42&amp;" "&amp;G43&amp;" "&amp;G44&amp;" "&amp;G45&amp;" "&amp;G46&amp;"-----SH: "&amp;G48&amp;" "&amp;G49&amp;" "&amp;G50&amp;" "&amp;G51&amp;" "&amp;G52&amp;" "&amp;G53&amp;" "&amp;G54&amp;" "&amp;G55&amp;" "&amp;G56&amp;" "&amp;G57&amp;"-----ROS: "&amp;G63&amp;" "&amp;G64&amp;" "&amp;G65&amp;" "&amp;G66&amp;" "&amp;G67&amp;" "&amp;G68&amp;" "&amp;G70&amp;" "&amp;G71&amp;" "&amp;G72&amp;" "&amp;G73&amp;" "&amp;G74&amp;" "&amp;G75&amp;" "&amp;G76&amp;" "&amp;G78&amp;" "&amp;G79&amp;" "&amp;G80&amp;" "&amp;G82&amp;" "&amp;G83&amp;" "&amp;G84&amp;" "&amp;G85&amp;" "&amp;G87&amp;" "&amp;G88&amp;" "&amp;G89&amp;" "&amp;G90&amp;" "&amp;G91&amp;" "&amp;G93&amp;" "&amp;G94&amp;" "&amp;G95&amp;" "&amp;G96&amp;" "&amp;G97&amp;" "&amp;G99&amp;" "&amp;G101&amp;" "&amp;G103&amp;" "&amp;G105&amp;" "&amp;G107&amp;" "&amp;G109&amp;" "&amp;G111&amp;" "&amp;G113&amp;" "&amp;G114&amp;"-----EXAM: "&amp;G133&amp;" "&amp;G134&amp;" "&amp;G135&amp;" "&amp;G137&amp;" "&amp;G138&amp;" "&amp;G139&amp;" "&amp;G141&amp;" "&amp;G151&amp;" "&amp;G164&amp;" "&amp;G167&amp;" "&amp;G168&amp;" "&amp;G173&amp;" "&amp;G175&amp;" "&amp;G177&amp;" "&amp;G179&amp;" "&amp;G181&amp;" "&amp;G183&amp;" "&amp;G185&amp;" "&amp;G187&amp;"----------"&amp;G196&amp;G197&amp;G198&amp;"  Psychotherapy included: "&amp;G201&amp;" "&amp;G202&amp;" "&amp;G203&amp;" "&amp;G204&amp;" "&amp;G205&amp;" "&amp;G207&amp;"."</f>
-        <v>CC:  Problems addressed in this encounter include .Additional workup planned (if any), includes: .Risk to patient is considered Minimal due to having only one minor (self-limiting) problem.MDM is High.-----HPI: Pt. has had  for .         -----PFSH: MEDICAL HISTORY::.:.:.0-----FH:0           -----SH: 0 Does not have a job. Does not have a car. Not born by C-section or does not know. Gallbladder has been removed. Has not had gastric bypass surgery. No developmental delays. PLEASE ELABORATE  -----ROS: Negative for hallucinations. Negative for SI. Negative for anxiety. Negative for insomnia. Negative for drug/alcohol abuse.  Constitutional:Negative for fatigue.              GI:Negative for nausea.                  All other systems reviewed and are negative.-----EXAM:    Inappropriately groomed and/or dressed PLEASE OVERRIDE TEXT HERE TO EXPLAIN Pt. has nutritional deficiencies. PLEASE OVERRIDE TEXT HERE TO EXPLAIN Has deformities relevant to mental status. OVERRIDE TEXT HERE TO EXPLAIN Speech is normal for  Thought content: . Associations are loose. Pt. confirms . Pt. denies SI/HI, hallucinations, delusions, obsessions, aggressive/violent ruminations.. Loose judgment/insight. OVERIDE TEXT HERE TO ELABORATE Recent and remote memory is loose. Attention span/concentration below average. OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE. Mood is , and affect congruent.----------  Psychotherapy included:      .</v>
+        <v>CC:  Problems addressed in this encounter include est problem, stable problem, .Additional workup planned (if any), includes: .Risk to patient is considered Moderate due to stopping, starting, or changing Rx (other than LiCo).MDM is High.-----HPI: Pt. has had  for .         -----PFSH: MEDICAL HISTORY::.:.:.0-----FH:0           -----SH: 0 Does not have a job. Does not have a car. Not born by C-section or does not know. Gallbladder has been removed. Has not had gastric bypass surgery. No developmental delays. PLEASE ELABORATE  -----ROS: Negative for hallucinations. Negative for SI. Negative for anxiety. Negative for insomnia. Negative for drug/alcohol abuse.  Constitutional:Negative for fatigue.              GI:Negative for nausea.                  All other systems reviewed and are negative.-----EXAM:    Inappropriately groomed and/or dressed PLEASE OVERRIDE TEXT HERE TO EXPLAIN Pt. has nutritional deficiencies. PLEASE OVERRIDE TEXT HERE TO EXPLAIN Has deformities relevant to mental status. OVERRIDE TEXT HERE TO EXPLAIN Speech is normal for  Thought content: . Associations are loose. Pt. confirms . Pt. denies SI/HI, hallucinations, delusions, obsessions, aggressive/violent ruminations.. Loose judgment/insight. OVERIDE TEXT HERE TO ELABORATE Recent and remote memory is loose. Attention span/concentration below average. OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE. Mood is , and affect congruent.----------  Psychotherapy included:      .</v>
       </c>
       <c r="B222" s="133"/>
       <c r="C222" s="133"/>
@@ -24312,7 +24336,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P236"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118:G118"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -28437,7 +28463,7 @@
     <row r="220" spans="1:16" s="39" customFormat="1" ht="180" customHeight="1">
       <c r="A220" s="133" t="str">
         <f>'MDM calculator'!N1&amp;G1&amp;"-----HPI: "&amp;G19&amp;" "&amp;G20&amp;" "&amp;G21&amp;" "&amp;G22&amp;" "&amp;G23&amp;" "&amp;G24&amp;" "&amp;G25&amp;" "&amp;G26&amp;"-----PFSH: MEDICAL HISTORY:"&amp;C11&amp;":"&amp;G11&amp;"."&amp;C12&amp;":"&amp;G12&amp;"."&amp;C13&amp;":"&amp;G13&amp;"."&amp;G31&amp;"-----FH:"&amp;G33&amp;" "&amp;G34&amp;" "&amp;G35&amp;" "&amp;G36&amp;" "&amp;G37&amp;" "&amp;G38&amp;" "&amp;G39&amp;" "&amp;G40&amp;" "&amp;G41&amp;" "&amp;G42&amp;" "&amp;G43&amp;" "&amp;G44&amp;"-----SH: "&amp;G46&amp;" "&amp;G47&amp;" "&amp;G48&amp;" "&amp;G49&amp;" "&amp;G50&amp;" "&amp;G51&amp;" "&amp;G52&amp;" "&amp;G53&amp;" "&amp;G54&amp;" "&amp;G55&amp;"-----ROS: "&amp;G61&amp;" "&amp;G62&amp;" "&amp;G63&amp;" "&amp;G64&amp;" "&amp;G65&amp;" "&amp;G66&amp;" "&amp;G68&amp;" "&amp;G69&amp;" "&amp;G70&amp;" "&amp;G71&amp;" "&amp;G72&amp;" "&amp;G73&amp;" "&amp;G74&amp;" "&amp;G76&amp;" "&amp;G77&amp;" "&amp;G78&amp;" "&amp;G80&amp;" "&amp;G81&amp;" "&amp;G82&amp;" "&amp;G83&amp;" "&amp;G85&amp;" "&amp;G86&amp;" "&amp;G87&amp;" "&amp;G88&amp;" "&amp;G89&amp;" "&amp;G91&amp;" "&amp;G92&amp;" "&amp;G93&amp;" "&amp;G94&amp;" "&amp;G95&amp;" "&amp;G97&amp;" "&amp;G99&amp;" "&amp;G101&amp;" "&amp;G103&amp;" "&amp;G105&amp;" "&amp;G107&amp;" "&amp;G109&amp;" "&amp;G111&amp;" "&amp;G112&amp;"-----EXAM: "&amp;G131&amp;" "&amp;G132&amp;" "&amp;G133&amp;" "&amp;G135&amp;" "&amp;G136&amp;" "&amp;G137&amp;" "&amp;G139&amp;" "&amp;G149&amp;" "&amp;G162&amp;" "&amp;G165&amp;" "&amp;G166&amp;" "&amp;G171&amp;" "&amp;G173&amp;" "&amp;G175&amp;" "&amp;G177&amp;" "&amp;G179&amp;" "&amp;G181&amp;" "&amp;G183&amp;" "&amp;G185&amp;"----------"&amp;G199&amp;G200&amp;G201&amp;"  Psychotherapy included: "&amp;G204&amp;" "&amp;G205&amp;" "&amp;G206&amp;" "&amp;G207&amp;" "&amp;G208&amp;" "&amp;G210&amp;"."</f>
-        <v>CC:  Problems addressed in this encounter include .Additional workup planned (if any), includes: .Risk to patient is considered Minimal due to having only one minor (self-limiting) problem.MDM is Moderate.-----HPI: Pt. has had  for .         -----PFSH: MEDICAL HISTORY::.:.:.0-----FH:0           -----SH: 0 Does not have a job. Does not have a car. Not born by C-section or does not know. Gallbladder has been removed. Has not had gastric bypass surgery. No developmental delays. PLEASE ELABORATE  -----ROS: Negative for hallucinations. Negative for SI. Negative for anxiety. Negative for insomnia. Negative for drug/alcohol abuse.  Constitutional:Negative for fatigue.              GI:Negative for nausea.                  All other systems reviewed and are negative.-----EXAM:    Inappropriately groomed and/or dressed PLEASE OVERRIDE TEXT HERE TO EXPLAIN Pt. has nutritional deficiencies. PLEASE OVERRIDE TEXT HERE TO EXPLAIN Has deformities relevant to mental status. OVERRIDE TEXT HERE TO EXPLAIN Speech is normal for  Thought content: . Associations are loose. Pt. confirms . Pt. denies SI/HI, hallucinations, delusions, obsessions, aggressive/violent ruminations.. Loose judgment/insight. OVERIDE TEXT HERE TO ELABORATE Recent and remote memory is loose. Attention span/concentration below average. OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE. ----------  Psychotherapy included:      .</v>
+        <v>CC:  Problems addressed in this encounter include est problem, stable problem, .Additional workup planned (if any), includes: .Risk to patient is considered Moderate due to stopping, starting, or changing Rx (other than LiCo).MDM is Moderate.-----HPI: Pt. has had  for .         -----PFSH: MEDICAL HISTORY::.:.:.0-----FH:0           -----SH: 0 Does not have a job. Does not have a car. Not born by C-section or does not know. Gallbladder has been removed. Has not had gastric bypass surgery. No developmental delays. PLEASE ELABORATE  -----ROS: Negative for hallucinations. Negative for SI. Negative for anxiety. Negative for insomnia. Negative for drug/alcohol abuse.  Constitutional:Negative for fatigue.              GI:Negative for nausea.                  All other systems reviewed and are negative.-----EXAM:    Inappropriately groomed and/or dressed PLEASE OVERRIDE TEXT HERE TO EXPLAIN Pt. has nutritional deficiencies. PLEASE OVERRIDE TEXT HERE TO EXPLAIN Has deformities relevant to mental status. OVERRIDE TEXT HERE TO EXPLAIN Speech is normal for  Thought content: . Associations are loose. Pt. confirms . Pt. denies SI/HI, hallucinations, delusions, obsessions, aggressive/violent ruminations.. Loose judgment/insight. OVERIDE TEXT HERE TO ELABORATE Recent and remote memory is loose. Attention span/concentration below average. OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE. ----------  Psychotherapy included:      .</v>
       </c>
       <c r="B220" s="133"/>
       <c r="C220" s="133"/>
@@ -28788,7 +28814,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P229"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110:G110"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
@@ -32826,7 +32854,7 @@
     <row r="213" spans="1:16" s="39" customFormat="1" ht="180" customHeight="1">
       <c r="A213" s="133" t="str">
         <f>'MDM calculator'!N1&amp;G1&amp;"-----HPI: "&amp;G11&amp;" "&amp;G12&amp;" "&amp;G13&amp;" "&amp;G14&amp;" "&amp;G15&amp;" "&amp;G16&amp;" "&amp;G17&amp;" "&amp;G18&amp;"-----PFSH: MEDICAL HISTORY:"&amp;G23&amp;"-----FH:"&amp;G25&amp;" "&amp;G26&amp;" "&amp;G27&amp;" "&amp;G28&amp;" "&amp;G29&amp;" "&amp;G30&amp;" "&amp;G31&amp;" "&amp;G32&amp;" "&amp;G33&amp;" "&amp;G34&amp;" "&amp;G35&amp;" "&amp;G36&amp;"-----SH: "&amp;G38&amp;" "&amp;G39&amp;" "&amp;G40&amp;" "&amp;G41&amp;" "&amp;G42&amp;" "&amp;G43&amp;" "&amp;G44&amp;" "&amp;G45&amp;" "&amp;G46&amp;" "&amp;G47&amp;"-----ROS: "&amp;G53&amp;" "&amp;G54&amp;" "&amp;G55&amp;" "&amp;G56&amp;" "&amp;G57&amp;" "&amp;G58&amp;" "&amp;G60&amp;" "&amp;G61&amp;" "&amp;G62&amp;" "&amp;G63&amp;" "&amp;G64&amp;" "&amp;G65&amp;" "&amp;G66&amp;" "&amp;G68&amp;" "&amp;G69&amp;" "&amp;G70&amp;" "&amp;G72&amp;" "&amp;G73&amp;" "&amp;G74&amp;" "&amp;G75&amp;" "&amp;G77&amp;" "&amp;G78&amp;" "&amp;G79&amp;" "&amp;G80&amp;" "&amp;G81&amp;" "&amp;G83&amp;" "&amp;G84&amp;" "&amp;G85&amp;" "&amp;G86&amp;" "&amp;G87&amp;" "&amp;G89&amp;" "&amp;G91&amp;" "&amp;G93&amp;" "&amp;G95&amp;" "&amp;G97&amp;" "&amp;G99&amp;" "&amp;G101&amp;" "&amp;G103&amp;" "&amp;G104&amp;"-----EXAM: "&amp;G123&amp;" "&amp;G124&amp;" "&amp;G125&amp;" "&amp;G127&amp;" "&amp;G128&amp;" "&amp;G129&amp;" "&amp;G131&amp;" "&amp;G141&amp;" "&amp;G154&amp;" "&amp;G157&amp;" "&amp;G158&amp;" "&amp;G163&amp;" "&amp;G165&amp;" "&amp;G167&amp;" "&amp;G169&amp;" "&amp;G171&amp;" "&amp;G173&amp;" "&amp;G175&amp;" "&amp;G177&amp;"----------"&amp;G192&amp;G193&amp;G194&amp;"  Psychotherapy included: "&amp;G197&amp;" "&amp;G198&amp;" "&amp;G199&amp;" "&amp;G200&amp;" "&amp;G201&amp;" "&amp;G203&amp;"."</f>
-        <v>CC:  Problems addressed in this encounter include .Additional workup planned (if any), includes: .Risk to patient is considered Minimal due to having only one minor (self-limiting) problem.MDM is Low.-----HPI: Pt. has had  for .         -----PFSH: MEDICAL HISTORY:0-----FH:0           -----SH: 0 Does not have a job. Does not have a car. Not born by C-section or does not know. Gallbladder has been removed. Has not had gastric bypass surgery. No developmental delays. PLEASE ELABORATE  -----ROS: Negative for hallucinations. Negative for SI. Negative for anxiety. Negative for insomnia. Negative for drug/alcohol abuse.  Constitutional:Negative for fatigue.              GI:Negative for nausea.                  All other systems reviewed and are negative.-----EXAM:    Inappropriately groomed and/or dressed PLEASE OVERRIDE TEXT HERE TO EXPLAIN Pt. has nutritional deficiencies. PLEASE OVERRIDE TEXT HERE TO EXPLAIN Has deformities relevant to mental status. OVERRIDE TEXT HERE TO EXPLAIN Speech is normal for  Thought content: . Associations are loose. Pt. confirms . Pt. denies SI/HI, hallucinations, delusions, obsessions, aggressive/violent ruminations.. Loose judgment/insight. OVERIDE TEXT HERE TO ELABORATE Recent and remote memory is loose. Attention span/concentration below average. OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE. ----------  Psychotherapy included:      .</v>
+        <v>CC:  Problems addressed in this encounter include est problem, stable problem, .Additional workup planned (if any), includes: .Risk to patient is considered Moderate due to stopping, starting, or changing Rx (other than LiCo).MDM is Low.-----HPI: Pt. has had  for .         -----PFSH: MEDICAL HISTORY:0-----FH:0           -----SH: 0 Does not have a job. Does not have a car. Not born by C-section or does not know. Gallbladder has been removed. Has not had gastric bypass surgery. No developmental delays. PLEASE ELABORATE  -----ROS: Negative for hallucinations. Negative for SI. Negative for anxiety. Negative for insomnia. Negative for drug/alcohol abuse.  Constitutional:Negative for fatigue.              GI:Negative for nausea.                  All other systems reviewed and are negative.-----EXAM:    Inappropriately groomed and/or dressed PLEASE OVERRIDE TEXT HERE TO EXPLAIN Pt. has nutritional deficiencies. PLEASE OVERRIDE TEXT HERE TO EXPLAIN Has deformities relevant to mental status. OVERRIDE TEXT HERE TO EXPLAIN Speech is normal for  Thought content: . Associations are loose. Pt. confirms . Pt. denies SI/HI, hallucinations, delusions, obsessions, aggressive/violent ruminations.. Loose judgment/insight. OVERIDE TEXT HERE TO ELABORATE Recent and remote memory is loose. Attention span/concentration below average. OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE OVERIDE TEXT HERE TO ELABORATE. ----------  Psychotherapy included:      .</v>
       </c>
       <c r="B213" s="133"/>
       <c r="C213" s="133"/>

</xml_diff>

<commit_message>
changed text on two fields to remove ambiguity from old version of calculator, per note from client
</commit_message>
<xml_diff>
--- a/clientdocs/Mike calculator v2.xlsx
+++ b/clientdocs/Mike calculator v2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27810" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27810" windowHeight="12195" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="MDM calculator" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="259">
   <si>
     <t>Medical Decision Making - Problems being addressed, data being reviewed, risk to patient.</t>
   </si>
@@ -710,9 +710,6 @@
     <t>Or, you may bill based on 25 minutes time, only if you do not bill add-on code for psychotherapy.</t>
   </si>
   <si>
-    <t>For this returning patient, you either need to update HPI, or you can update the status of 3 chronic or inactive conditions. Pick one "+" in the left margin.</t>
-  </si>
-  <si>
     <t>Or, you may bill based on 40 minutes time, only if you do not bill add-on code for psychotherapy.</t>
   </si>
   <si>
@@ -898,6 +895,12 @@
   </si>
   <si>
     <t>stable problem</t>
+  </si>
+  <si>
+    <t>For this returning patient, you either need to update HPI, or you can update the status of 3 chronic or inactive conditions.</t>
+  </si>
+  <si>
+    <t>For this returning patient, you either need to update HPI, or you can update the status of 3 chronic or inactive conditions</t>
   </si>
 </sst>
 </file>
@@ -2293,7 +2296,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2304,7 +2307,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2421,7 +2424,7 @@
     </row>
     <row r="5" spans="1:25" s="3" customFormat="1">
       <c r="A5" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -2495,7 +2498,7 @@
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>7</v>
@@ -2578,7 +2581,7 @@
       <c r="G11" s="128"/>
       <c r="H11" s="13"/>
       <c r="K11" s="64" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L11" s="13" t="str">
         <f>K8</f>
@@ -2594,7 +2597,7 @@
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G12" s="128" t="str">
         <f t="shared" ref="G12:G24" si="0" xml:space="preserve"> IF(ISTEXT(F12),", ","")</f>
@@ -2605,7 +2608,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="64" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L12" s="13" t="str">
         <f>K9</f>
@@ -2621,7 +2624,7 @@
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G13" s="128" t="str">
         <f t="shared" si="0"/>
@@ -2632,7 +2635,7 @@
         <v>1</v>
       </c>
       <c r="K13" s="64" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L13" s="13" t="str">
         <f>K7</f>
@@ -2657,7 +2660,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="64" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L14" s="13" t="str">
         <f>K8</f>
@@ -2682,7 +2685,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="64" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L15" s="13" t="str">
         <f>K8</f>
@@ -2707,7 +2710,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="64" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L16" s="13" t="str">
         <f>K8</f>
@@ -2724,7 +2727,7 @@
       <c r="G17" s="128"/>
       <c r="H17" s="13"/>
       <c r="K17" s="64" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L17" s="13" t="str">
         <f>K9</f>
@@ -2749,7 +2752,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="64" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L18" s="13" t="str">
         <f>K9</f>
@@ -2774,7 +2777,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="64" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L19" s="13" t="str">
         <f>K9</f>
@@ -2799,7 +2802,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="64" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L20" s="13" t="str">
         <f>K6</f>
@@ -2878,7 +2881,7 @@
       <c r="E25" s="13"/>
       <c r="F25" s="128"/>
       <c r="G25" s="128" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H25" s="13"/>
     </row>
@@ -3205,7 +3208,7 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="64" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
@@ -3218,10 +3221,10 @@
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
       <c r="F48" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -3234,7 +3237,7 @@
         <v>Moderate</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -3481,7 +3484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P223"/>
   <sheetViews>
-    <sheetView topLeftCell="A184" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A207" sqref="A207:G223"/>
     </sheetView>
   </sheetViews>
@@ -3507,7 +3510,7 @@
         <v>186</v>
       </c>
       <c r="G1" s="127" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -3573,7 +3576,7 @@
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="70" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D10" s="22"/>
       <c r="F10" s="22"/>
@@ -3585,7 +3588,7 @@
       </c>
       <c r="B11" s="29"/>
       <c r="C11" s="70" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D11" s="22"/>
       <c r="F11" s="22">
@@ -3611,7 +3614,7 @@
       </c>
       <c r="B12" s="45"/>
       <c r="C12" s="70" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D12" s="46"/>
       <c r="F12" s="22">
@@ -3637,7 +3640,7 @@
       </c>
       <c r="B13" s="45"/>
       <c r="C13" s="70" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D13" s="46"/>
       <c r="F13" s="22">
@@ -3663,7 +3666,7 @@
       </c>
       <c r="B14" s="45"/>
       <c r="C14" s="70" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D14" s="46"/>
       <c r="F14" s="22">
@@ -3689,7 +3692,7 @@
       </c>
       <c r="B15" s="45"/>
       <c r="C15" s="70" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D15" s="46"/>
       <c r="F15" s="22">
@@ -3715,7 +3718,7 @@
       </c>
       <c r="B16" s="45"/>
       <c r="C16" s="70" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D16" s="46"/>
       <c r="F16" s="22">
@@ -3741,7 +3744,7 @@
       </c>
       <c r="B17" s="29"/>
       <c r="C17" s="70" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D17" s="22"/>
       <c r="F17" s="22">
@@ -3759,7 +3762,7 @@
       </c>
       <c r="B18" s="73"/>
       <c r="C18" s="74" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D18" s="22"/>
       <c r="F18" s="22">
@@ -3856,7 +3859,7 @@
       </c>
       <c r="B23" s="76"/>
       <c r="C23" s="77" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D23" s="38"/>
       <c r="F23" s="22">
@@ -3898,7 +3901,7 @@
       </c>
       <c r="B25" s="79"/>
       <c r="C25" s="80" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D25" s="22"/>
       <c r="F25" s="22">
@@ -3924,7 +3927,7 @@
       </c>
       <c r="B26" s="29"/>
       <c r="C26" s="81" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D26" s="22"/>
       <c r="F26" s="22">
@@ -3950,7 +3953,7 @@
       </c>
       <c r="B27" s="29"/>
       <c r="C27" s="81" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D27" s="22"/>
       <c r="F27" s="22">
@@ -3976,7 +3979,7 @@
       </c>
       <c r="B28" s="29"/>
       <c r="C28" s="81" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D28" s="22"/>
       <c r="F28" s="22">
@@ -4002,7 +4005,7 @@
       </c>
       <c r="B29" s="29"/>
       <c r="C29" s="81" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D29" s="22"/>
       <c r="F29" s="22">
@@ -4028,7 +4031,7 @@
       </c>
       <c r="B30" s="29"/>
       <c r="C30" s="81" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D30" s="22"/>
       <c r="F30" s="22">
@@ -4054,7 +4057,7 @@
       </c>
       <c r="B31" s="29"/>
       <c r="C31" s="81" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D31" s="22"/>
       <c r="F31" s="22">
@@ -4080,7 +4083,7 @@
       </c>
       <c r="B32" s="29"/>
       <c r="C32" s="81" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D32" s="22"/>
       <c r="F32" s="22">
@@ -4106,7 +4109,7 @@
       </c>
       <c r="B33" s="29"/>
       <c r="C33" s="81" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D33" s="22"/>
       <c r="F33" s="22">
@@ -4132,7 +4135,7 @@
       </c>
       <c r="B34" s="29"/>
       <c r="C34" s="81" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D34" s="22"/>
       <c r="F34" s="22">
@@ -4158,7 +4161,7 @@
       </c>
       <c r="B35" s="29"/>
       <c r="C35" s="81" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D35" s="22"/>
       <c r="F35" s="22">
@@ -4184,7 +4187,7 @@
       </c>
       <c r="B36" s="73"/>
       <c r="C36" s="81" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D36" s="22"/>
       <c r="F36" s="22">
@@ -4229,7 +4232,7 @@
       </c>
       <c r="B38" s="83"/>
       <c r="C38" s="80" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D38" s="22"/>
       <c r="F38" s="22">
@@ -4394,7 +4397,7 @@
       </c>
       <c r="B46" s="29"/>
       <c r="C46" s="81" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D46" s="22"/>
       <c r="F46" s="22">
@@ -4412,7 +4415,7 @@
       </c>
       <c r="B47" s="73"/>
       <c r="C47" s="82" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D47" s="22"/>
       <c r="F47" s="22">
@@ -7197,7 +7200,7 @@
       <c r="E191" s="22"/>
       <c r="F191" s="22"/>
       <c r="G191" s="97" t="str">
-        <f xml:space="preserve"> IF(ISTEXT(B191),C191&amp;"/","")</f>
+        <f t="shared" ref="G191:G196" si="22" xml:space="preserve"> IF(ISTEXT(B191),C191&amp;"/","")</f>
         <v/>
       </c>
     </row>
@@ -7211,7 +7214,7 @@
       <c r="E192" s="22"/>
       <c r="F192" s="22"/>
       <c r="G192" s="97" t="str">
-        <f xml:space="preserve"> IF(ISTEXT(B192),C192&amp;"/","")</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
@@ -7225,7 +7228,7 @@
       <c r="E193" s="22"/>
       <c r="F193" s="22"/>
       <c r="G193" s="97" t="str">
-        <f xml:space="preserve"> IF(ISTEXT(B193),C193&amp;"/","")</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
@@ -7239,7 +7242,7 @@
       <c r="E194" s="22"/>
       <c r="F194" s="22"/>
       <c r="G194" s="97" t="str">
-        <f xml:space="preserve"> IF(ISTEXT(B194),C194&amp;"/","")</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
@@ -7253,7 +7256,7 @@
       <c r="E195" s="22"/>
       <c r="F195" s="22"/>
       <c r="G195" s="97" t="str">
-        <f xml:space="preserve"> IF(ISTEXT(B195),C195&amp;"/","")</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
@@ -7267,7 +7270,7 @@
       <c r="E196" s="22"/>
       <c r="F196" s="22"/>
       <c r="G196" s="97" t="str">
-        <f xml:space="preserve"> IF(ISTEXT(B196),C196&amp;"/","")</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
@@ -7275,13 +7278,13 @@
       <c r="A197" s="43"/>
       <c r="B197" s="101"/>
       <c r="C197" s="112" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D197" s="22"/>
       <c r="E197" s="22"/>
       <c r="F197" s="22"/>
       <c r="G197" s="119" t="str">
-        <f t="shared" ref="G197" si="22" xml:space="preserve"> IF(ISTEXT(B197),C197,"")</f>
+        <f t="shared" ref="G197" si="23" xml:space="preserve"> IF(ISTEXT(B197),C197,"")</f>
         <v/>
       </c>
     </row>
@@ -7606,7 +7609,7 @@
         <v>186</v>
       </c>
       <c r="G1" s="127" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -11638,7 +11641,7 @@
         <v>186</v>
       </c>
       <c r="G1" s="127" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -15749,7 +15752,7 @@
         <v>186</v>
       </c>
       <c r="G1" s="127" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -19831,8 +19834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P238"/>
   <sheetViews>
-    <sheetView topLeftCell="A120" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19850,17 +19853,17 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D1" s="18"/>
       <c r="E1" s="117"/>
       <c r="G1" s="127" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="18"/>
       <c r="D2" s="18"/>
@@ -19896,7 +19899,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="123" t="s">
-        <v>210</v>
+        <v>257</v>
       </c>
       <c r="B8" s="62"/>
       <c r="C8" s="26"/>
@@ -19916,7 +19919,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B10" s="38"/>
       <c r="C10" s="22"/>
@@ -19929,7 +19932,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B11" s="38"/>
       <c r="C11" s="112"/>
@@ -19938,12 +19941,12 @@
       <c r="F11" s="22"/>
       <c r="G11" s="25"/>
       <c r="I11" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B12" s="38"/>
       <c r="C12" s="112"/>
@@ -19952,12 +19955,12 @@
       <c r="F12" s="22"/>
       <c r="G12" s="25"/>
       <c r="I12" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B13" s="38"/>
       <c r="C13" s="112"/>
@@ -24336,8 +24339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P236"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118:G118"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24360,7 +24363,7 @@
       <c r="D1" s="18"/>
       <c r="E1" s="117"/>
       <c r="G1" s="127" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -24402,7 +24405,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="123" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="B8" s="62"/>
       <c r="C8" s="26"/>
@@ -24422,7 +24425,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B10" s="38"/>
       <c r="C10" s="22"/>
@@ -24435,7 +24438,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B11" s="38"/>
       <c r="C11" s="112"/>
@@ -24444,12 +24447,12 @@
       <c r="F11" s="22"/>
       <c r="G11" s="25"/>
       <c r="I11" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B12" s="38"/>
       <c r="C12" s="112"/>
@@ -24458,12 +24461,12 @@
       <c r="F12" s="22"/>
       <c r="G12" s="25"/>
       <c r="I12" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B13" s="38"/>
       <c r="C13" s="112"/>
@@ -28843,7 +28846,7 @@
         <v>186</v>
       </c>
       <c r="G1" s="127" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -29153,7 +29156,7 @@
       </c>
       <c r="B22" s="61"/>
       <c r="C22" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D22" s="37"/>
       <c r="F22" s="22"/>

</xml_diff>